<commit_message>
fix understanding OS ch 3
</commit_message>
<xml_diff>
--- a/data/prp_codebook.xlsx
+++ b/data/prp_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/gaby_mahrholz_glasgow_ac_uk/Documents/R_Book/analysis-v3-main/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/gaby_mahrholz_glasgow_ac_uk/Documents/R_Book/analysis-v3-main/data/data_pair_ch1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{A4BB619F-3534-4C83-B426-FC4CEF662815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814A248C-6C5D-4583-B351-2E5B66D88710}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{A4BB619F-3534-4C83-B426-FC4CEF662815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{987DD1AE-4A7C-4F37-8661-058BF96FA357}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{24A17B94-EE2B-4420-8906-A2267C65E0A0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{24A17B94-EE2B-4420-8906-A2267C65E0A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,22 +666,22 @@
 </t>
   </si>
   <si>
+    <t>How confident are you in your ability to explain these concepts? 1 (Not at all confident) to 7 (Entirely confident)
+Understanding_OS_X_Time1 = T1
+Understanding_OS_X_Time2 = T2
+Understanding_OS needs to be averaged</t>
+  </si>
+  <si>
     <t xml:space="preserve">To what extent do you view the following practices as sensible (1) to problematic (7) for your research: (Likert scale from Sensible [1] to Problematic [7])
 Measured at 2 timepoints:
-QRPs_1 = T1
-QRPs_1_Time2 = T2 (In this reduced dataset, QRPs at T2 has already been averaged)
+QRPs_X_Time1 = T1
+QRPs_X_Time2 = T2 (In this reduced dataset, QRPs at T2 has already been averaged)
 We computed all 11 items pertaining to QRPs into one total indicating general acceptance of QRPs such that higher scores indicate less acceptance of QRPs.
 </t>
   </si>
   <si>
-    <t>How confident are you in your ability to explain these concepts? 1 (Not at all confident) to 7 (Entirely confident)
-Understanding_OS_Time1 = T1
-Understanding_OS_1_Time2 = T2
-Understanding_OS needs to be averaged</t>
-  </si>
-  <si>
     <t>scale from 1 (strongly disagree) to 5
-(strongly agree). Answers were aggregated into one overall
+(strongly agree). Typo in the paper where it says 1-5. Answers were aggregated into one overall
 score of supervisory support
 15 is Reverse-scored and then all items averaged. In the original dataset, that was already computed, yet here we reversed the action and present to you the participants response to the question rather than the corrected score. Item 15 needs to be reverse-scored before you can compute the average</t>
   </si>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44440229-DC2E-4044-9CA4-16EB38FD6499}">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,7 +1726,7 @@
         <v>71</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>69</v>
@@ -1955,7 +1955,7 @@
         <v>91</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>37</v>

</xml_diff>